<commit_message>
Changes OrangeHRM test case as Yes
</commit_message>
<xml_diff>
--- a/KeywordFramework/TestCase.xlsx
+++ b/KeywordFramework/TestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2850" windowWidth="14415" windowHeight="2790"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="14415" windowHeight="2415"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -480,7 +480,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -488,7 +488,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>